<commit_message>
Added model for HL cover, created plots for significant env variables
</commit_message>
<xml_diff>
--- a/Result Tables/Model.result.tables_2024.xlsx
+++ b/Result Tables/Model.result.tables_2024.xlsx
@@ -6,13 +6,13 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="leaf.area" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="HL_cover" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t xml:space="preserve"/>
   </si>
@@ -32,7 +32,22 @@
     <t xml:space="preserve">(Intercept)</t>
   </si>
   <si>
+    <t xml:space="preserve">management2entbuscht</t>
+  </si>
+  <si>
+    <t xml:space="preserve">management2Buche</t>
+  </si>
+  <si>
+    <t xml:space="preserve">management2Fichte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SL_cover</t>
+  </si>
+  <si>
     <t xml:space="preserve">soil_cover</t>
+  </si>
+  <si>
+    <t xml:space="preserve">moss_cover</t>
   </si>
 </sst>
 </file>
@@ -412,13 +427,13 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>109.002</v>
+        <v>90.767</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>4.677</v>
+        <v>9.303</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>23.304</v>
+        <v>9.756</v>
       </c>
       <c r="E2" s="2" t="n">
         <v>0</v>
@@ -429,16 +444,101 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>-0.368</v>
+        <v>-12.613</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>0.152</v>
+        <v>5.588</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>-2.425</v>
+        <v>-2.257</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>0.0176</v>
+        <v>0.027</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>-9.471</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>5.771</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>-1.641</v>
+      </c>
+      <c r="E4" s="2" t="n">
+        <v>0.1051</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>-35.861</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>6.39</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>-5.612</v>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>-0.202</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>-2.245</v>
+      </c>
+      <c r="E6" s="2" t="n">
+        <v>0.0278</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>-0.564</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>-4.689</v>
+      </c>
+      <c r="E7" s="2" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="2" t="n">
+        <v>-0.247</v>
+      </c>
+      <c r="C8" s="2" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D8" s="2" t="n">
+        <v>-2.473</v>
+      </c>
+      <c r="E8" s="2" t="n">
+        <v>0.0157</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
- merged 19+24 data - recreated models from 2024 analysis - plotted significant env variables
</commit_message>
<xml_diff>
--- a/Result Tables/Model.result.tables_2024.xlsx
+++ b/Result Tables/Model.result.tables_2024.xlsx
@@ -6,14 +6,14 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="nb.stem" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="area.bunch" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="prop.flower" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="nb.flower" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="stem.height" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="stem.per.sqm" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="leaf.area" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="HL_cover" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="nb.stem" sheetId="2" state="visible" r:id="rId1"/>
+    <sheet name="area.bunch" sheetId="3" state="visible" r:id="rId2"/>
+    <sheet name="prop.flower" sheetId="4" state="visible" r:id="rId3"/>
+    <sheet name="nb.flower" sheetId="5" state="visible" r:id="rId4"/>
+    <sheet name="stem.height" sheetId="6" state="visible" r:id="rId5"/>
+    <sheet name="stem.per.sqm" sheetId="7" state="visible" r:id="rId6"/>
+    <sheet name="leaf.area" sheetId="8" state="visible" r:id="rId7"/>
+    <sheet name="HL_cover" sheetId="9" state="visible" r:id="rId8"/>
   </sheets>
 </workbook>
 </file>
@@ -39,6 +39,12 @@
     <t xml:space="preserve">(Intercept)</t>
   </si>
   <si>
+    <t xml:space="preserve">soil_depth</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HL_cover</t>
+  </si>
+  <si>
     <t xml:space="preserve">management2entbuscht</t>
   </si>
   <si>
@@ -51,9 +57,6 @@
     <t xml:space="preserve">exposition</t>
   </si>
   <si>
-    <t xml:space="preserve">HL_cover</t>
-  </si>
-  <si>
     <t xml:space="preserve">TL_cover</t>
   </si>
   <si>
@@ -61,9 +64,6 @@
   </si>
   <si>
     <t xml:space="preserve">Pr(&gt;|t|)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">soil_depth</t>
   </si>
   <si>
     <t xml:space="preserve">soil_water</t>
@@ -478,7 +478,7 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B3" s="2" t="n">
         <v>0.373</v>
@@ -495,7 +495,7 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B4" s="2" t="n">
         <v>-2.839</v>
@@ -512,7 +512,7 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B5" s="2" t="n">
         <v>-0.255</v>
@@ -529,7 +529,7 @@
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B6" s="2" t="n">
         <v>0.015</v>
@@ -546,7 +546,7 @@
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B7" s="2" t="n">
         <v>0.011</v>
@@ -563,7 +563,7 @@
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B8" s="2" t="n">
         <v>-0.012</v>
@@ -603,10 +603,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2">
@@ -628,7 +628,7 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="B3" s="2" t="n">
         <v>-0.042</v>
@@ -645,7 +645,7 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B4" s="2" t="n">
         <v>0.013</v>
@@ -685,10 +685,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2">
@@ -710,7 +710,7 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B3" s="2" t="n">
         <v>-5.341</v>
@@ -727,7 +727,7 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B4" s="2" t="n">
         <v>1.178</v>
@@ -744,7 +744,7 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B5" s="2" t="n">
         <v>-0.593</v>
@@ -809,7 +809,7 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B3" s="2" t="n">
         <v>-0.65</v>
@@ -826,7 +826,7 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B4" s="2" t="n">
         <v>0.181</v>
@@ -843,7 +843,7 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B5" s="2" t="n">
         <v>0.005</v>
@@ -877,7 +877,7 @@
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B7" s="2" t="n">
         <v>0.014</v>
@@ -917,10 +917,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2">
@@ -982,10 +982,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2">
@@ -1007,7 +1007,7 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B3" s="2" t="n">
         <v>78.497</v>
@@ -1024,7 +1024,7 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B4" s="2" t="n">
         <v>14.898</v>
@@ -1041,7 +1041,7 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B5" s="2" t="n">
         <v>11.618</v>
@@ -1098,10 +1098,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2">
@@ -1163,10 +1163,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2">
@@ -1188,7 +1188,7 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B3" s="2" t="n">
         <v>-12.613</v>
@@ -1205,7 +1205,7 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B4" s="2" t="n">
         <v>-9.471</v>
@@ -1222,7 +1222,7 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B5" s="2" t="n">
         <v>-35.861</v>

</xml_diff>

<commit_message>
Transformed script into Quarto document. Minor changes in script itself
</commit_message>
<xml_diff>
--- a/Result Tables/Model.result.tables_2024.xlsx
+++ b/Result Tables/Model.result.tables_2024.xlsx
@@ -6,14 +6,14 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="nb.stem" sheetId="2" state="visible" r:id="rId1"/>
-    <sheet name="area.bunch" sheetId="3" state="visible" r:id="rId2"/>
-    <sheet name="prop.flower" sheetId="4" state="visible" r:id="rId3"/>
-    <sheet name="nb.flower" sheetId="5" state="visible" r:id="rId4"/>
-    <sheet name="stem.height" sheetId="6" state="visible" r:id="rId5"/>
-    <sheet name="stem.per.sqm" sheetId="7" state="visible" r:id="rId6"/>
-    <sheet name="leaf.area" sheetId="8" state="visible" r:id="rId7"/>
-    <sheet name="HL_cover" sheetId="9" state="visible" r:id="rId8"/>
+    <sheet name="nb.stem" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="area.bunch" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="prop.flower" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="nb.flower" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="stem.height" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="stem.per.sqm" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="leaf.area" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="HL_cover" sheetId="8" state="visible" r:id="rId8"/>
   </sheets>
 </workbook>
 </file>
@@ -39,31 +39,31 @@
     <t xml:space="preserve">(Intercept)</t>
   </si>
   <si>
+    <t xml:space="preserve">management2entbuscht</t>
+  </si>
+  <si>
+    <t xml:space="preserve">management2Buche</t>
+  </si>
+  <si>
+    <t xml:space="preserve">management2Fichte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">exposition</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HL_cover</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TL_cover</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pr(&gt;|t|)</t>
+  </si>
+  <si>
     <t xml:space="preserve">soil_depth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HL_cover</t>
-  </si>
-  <si>
-    <t xml:space="preserve">management2entbuscht</t>
-  </si>
-  <si>
-    <t xml:space="preserve">management2Buche</t>
-  </si>
-  <si>
-    <t xml:space="preserve">management2Fichte</t>
-  </si>
-  <si>
-    <t xml:space="preserve">exposition</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TL_cover</t>
-  </si>
-  <si>
-    <t xml:space="preserve">t value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pr(&gt;|t|)</t>
   </si>
   <si>
     <t xml:space="preserve">soil_water</t>
@@ -478,7 +478,7 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B3" s="2" t="n">
         <v>0.373</v>
@@ -495,7 +495,7 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4" s="2" t="n">
         <v>-2.839</v>
@@ -512,7 +512,7 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B5" s="2" t="n">
         <v>-0.255</v>
@@ -529,7 +529,7 @@
     </row>
     <row r="6">
       <c r="A6" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B6" s="2" t="n">
         <v>0.015</v>
@@ -546,7 +546,7 @@
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B7" s="2" t="n">
         <v>0.011</v>
@@ -563,7 +563,7 @@
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B8" s="2" t="n">
         <v>-0.012</v>
@@ -603,10 +603,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2">
@@ -628,7 +628,7 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B3" s="2" t="n">
         <v>-0.042</v>
@@ -645,7 +645,7 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B4" s="2" t="n">
         <v>0.013</v>
@@ -685,10 +685,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2">
@@ -710,7 +710,7 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B3" s="2" t="n">
         <v>-5.341</v>
@@ -727,7 +727,7 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4" s="2" t="n">
         <v>1.178</v>
@@ -744,7 +744,7 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B5" s="2" t="n">
         <v>-0.593</v>
@@ -809,7 +809,7 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B3" s="2" t="n">
         <v>-0.65</v>
@@ -826,7 +826,7 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4" s="2" t="n">
         <v>0.181</v>
@@ -843,7 +843,7 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B5" s="2" t="n">
         <v>0.005</v>
@@ -877,7 +877,7 @@
     </row>
     <row r="7">
       <c r="A7" s="2" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B7" s="2" t="n">
         <v>0.014</v>
@@ -917,10 +917,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2">
@@ -982,10 +982,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2">
@@ -1007,7 +1007,7 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B3" s="2" t="n">
         <v>78.497</v>
@@ -1024,7 +1024,7 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4" s="2" t="n">
         <v>14.898</v>
@@ -1041,7 +1041,7 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B5" s="2" t="n">
         <v>11.618</v>
@@ -1098,10 +1098,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2">
@@ -1163,10 +1163,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="2">
@@ -1188,7 +1188,7 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B3" s="2" t="n">
         <v>-12.613</v>
@@ -1205,7 +1205,7 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4" s="2" t="n">
         <v>-9.471</v>
@@ -1222,7 +1222,7 @@
     </row>
     <row r="5">
       <c r="A5" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B5" s="2" t="n">
         <v>-35.861</v>

</xml_diff>

<commit_message>
print models in quarto
</commit_message>
<xml_diff>
--- a/Result Tables/Model.result.tables_2024.xlsx
+++ b/Result Tables/Model.result.tables_2024.xlsx
@@ -8,12 +8,11 @@
   <sheets>
     <sheet name="nb.stem" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="area.bunch" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="prop.flower" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="nb.flower" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="stem.height" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="stem.per.sqm" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="leaf.area" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="HL_cover" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="nb.flower" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="stem.height" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="stem.per.sqm" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="leaf.area" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="HL_cover" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
 </workbook>
 </file>
@@ -685,10 +684,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2">
@@ -696,16 +695,16 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>0.189</v>
+        <v>-0.092</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>1.468</v>
+        <v>0.655</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>0.129</v>
+        <v>-0.141</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>0.8979</v>
+        <v>0.8879</v>
       </c>
     </row>
     <row r="3">
@@ -713,16 +712,16 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>-5.341</v>
+        <v>-0.65</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>2.077</v>
+        <v>0.234</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>-2.572</v>
+        <v>-2.779</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>0.0121</v>
+        <v>0.0054</v>
       </c>
     </row>
     <row r="4">
@@ -730,16 +729,16 @@
         <v>7</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>1.178</v>
+        <v>0.181</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>2.077</v>
+        <v>0.286</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>0.567</v>
+        <v>0.632</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>0.5721</v>
+        <v>0.5276</v>
       </c>
     </row>
     <row r="5">
@@ -747,16 +746,50 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="n">
-        <v>-0.593</v>
+        <v>0.005</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>2.077</v>
+        <v>0.372</v>
       </c>
       <c r="D5" s="2" t="n">
-        <v>-0.285</v>
+        <v>0.014</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>0.7762</v>
+        <v>0.9887</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>-0.043</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>0.022</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>-2.017</v>
+      </c>
+      <c r="E6" s="2" t="n">
+        <v>0.0437</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>0.014</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>2.612</v>
+      </c>
+      <c r="E7" s="2" t="n">
+        <v>0.009</v>
       </c>
     </row>
   </sheetData>
@@ -784,10 +817,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2">
@@ -795,101 +828,33 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>-0.092</v>
+        <v>3.331</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>0.655</v>
+        <v>0.073</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>-0.141</v>
+        <v>45.891</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>0.8879</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>-0.65</v>
+        <v>-0.004</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>0.234</v>
+        <v>0.002</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>-2.779</v>
+        <v>-1.642</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>0.0054</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="2" t="n">
-        <v>0.181</v>
-      </c>
-      <c r="C4" s="2" t="n">
-        <v>0.286</v>
-      </c>
-      <c r="D4" s="2" t="n">
-        <v>0.632</v>
-      </c>
-      <c r="E4" s="2" t="n">
-        <v>0.5276</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="2" t="n">
-        <v>0.005</v>
-      </c>
-      <c r="C5" s="2" t="n">
-        <v>0.372</v>
-      </c>
-      <c r="D5" s="2" t="n">
-        <v>0.014</v>
-      </c>
-      <c r="E5" s="2" t="n">
-        <v>0.9887</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="2" t="n">
-        <v>-0.043</v>
-      </c>
-      <c r="C6" s="2" t="n">
-        <v>0.022</v>
-      </c>
-      <c r="D6" s="2" t="n">
-        <v>-2.017</v>
-      </c>
-      <c r="E6" s="2" t="n">
-        <v>0.0437</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="2" t="n">
-        <v>0.014</v>
-      </c>
-      <c r="C7" s="2" t="n">
-        <v>0.005</v>
-      </c>
-      <c r="D7" s="2" t="n">
-        <v>2.612</v>
-      </c>
-      <c r="E7" s="2" t="n">
-        <v>0.009</v>
+        <v>0.1047</v>
       </c>
     </row>
   </sheetData>
@@ -928,33 +893,84 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>3.331</v>
+        <v>-7.397</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>0.073</v>
+        <v>23.907</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>45.891</v>
+        <v>-0.309</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>0</v>
+        <v>0.7579</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>-0.004</v>
+        <v>78.497</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>0.002</v>
+        <v>24.344</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>-1.642</v>
+        <v>3.225</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>0.1047</v>
+        <v>0.0019</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>14.898</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>23.965</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>0.622</v>
+      </c>
+      <c r="E4" s="2" t="n">
+        <v>0.5361</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>11.618</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>24.434</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>0.475</v>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>0.6358</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>3.754</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>0.923</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>4.066</v>
+      </c>
+      <c r="E6" s="2" t="n">
+        <v>0.0001</v>
       </c>
     </row>
   </sheetData>
@@ -993,84 +1009,33 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>-7.397</v>
+        <v>109.002</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>23.907</v>
+        <v>4.677</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>-0.309</v>
+        <v>23.304</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>0.7579</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>78.497</v>
+        <v>-0.368</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>24.344</v>
+        <v>0.152</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>3.225</v>
+        <v>-2.425</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>0.0019</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="2" t="n">
-        <v>14.898</v>
-      </c>
-      <c r="C4" s="2" t="n">
-        <v>23.965</v>
-      </c>
-      <c r="D4" s="2" t="n">
-        <v>0.622</v>
-      </c>
-      <c r="E4" s="2" t="n">
-        <v>0.5361</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="2" t="n">
-        <v>11.618</v>
-      </c>
-      <c r="C5" s="2" t="n">
-        <v>24.434</v>
-      </c>
-      <c r="D5" s="2" t="n">
-        <v>0.475</v>
-      </c>
-      <c r="E5" s="2" t="n">
-        <v>0.6358</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="2" t="n">
-        <v>3.754</v>
-      </c>
-      <c r="C6" s="2" t="n">
-        <v>0.923</v>
-      </c>
-      <c r="D6" s="2" t="n">
-        <v>4.066</v>
-      </c>
-      <c r="E6" s="2" t="n">
-        <v>0.0001</v>
+        <v>0.0176</v>
       </c>
     </row>
   </sheetData>
@@ -1088,71 +1053,6 @@
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="2" t="n">
-        <v>109.002</v>
-      </c>
-      <c r="C2" s="2" t="n">
-        <v>4.677</v>
-      </c>
-      <c r="D2" s="2" t="n">
-        <v>23.304</v>
-      </c>
-      <c r="E2" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="2" t="n">
-        <v>-0.368</v>
-      </c>
-      <c r="C3" s="2" t="n">
-        <v>0.152</v>
-      </c>
-      <c r="D3" s="2" t="n">
-        <v>-2.425</v>
-      </c>
-      <c r="E3" s="2" t="n">
-        <v>0.0176</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
-  <sheetData>
-    <row r="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
add corrmatrix to quarto
</commit_message>
<xml_diff>
--- a/Result Tables/Model.result.tables_2024.xlsx
+++ b/Result Tables/Model.result.tables_2024.xlsx
@@ -8,12 +8,11 @@
   <sheets>
     <sheet name="nb.stem" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="area.bunch" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="prop.flower" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="nb.flower" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="stem.height" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="stem.per.sqm" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="leaf.area" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="HL_cover" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="nb.flower" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="stem.height" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="stem.per.sqm" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="leaf.area" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="HL_cover" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
 </workbook>
 </file>
@@ -685,10 +684,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2">
@@ -696,16 +695,16 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>0.189</v>
+        <v>-0.092</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>1.468</v>
+        <v>0.655</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>0.129</v>
+        <v>-0.141</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>0.8979</v>
+        <v>0.8879</v>
       </c>
     </row>
     <row r="3">
@@ -713,16 +712,16 @@
         <v>6</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>-5.341</v>
+        <v>-0.65</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>2.077</v>
+        <v>0.234</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>-2.572</v>
+        <v>-2.779</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>0.0121</v>
+        <v>0.0054</v>
       </c>
     </row>
     <row r="4">
@@ -730,16 +729,16 @@
         <v>7</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>1.178</v>
+        <v>0.181</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>2.077</v>
+        <v>0.286</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>0.567</v>
+        <v>0.632</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>0.5721</v>
+        <v>0.5276</v>
       </c>
     </row>
     <row r="5">
@@ -747,16 +746,50 @@
         <v>8</v>
       </c>
       <c r="B5" s="2" t="n">
-        <v>-0.593</v>
+        <v>0.005</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>2.077</v>
+        <v>0.372</v>
       </c>
       <c r="D5" s="2" t="n">
-        <v>-0.285</v>
+        <v>0.014</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>0.7762</v>
+        <v>0.9887</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>-0.043</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>0.022</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>-2.017</v>
+      </c>
+      <c r="E6" s="2" t="n">
+        <v>0.0437</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="2" t="n">
+        <v>0.014</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="D7" s="2" t="n">
+        <v>2.612</v>
+      </c>
+      <c r="E7" s="2" t="n">
+        <v>0.009</v>
       </c>
     </row>
   </sheetData>
@@ -784,10 +817,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2">
@@ -795,101 +828,33 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>-0.092</v>
+        <v>3.331</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>0.655</v>
+        <v>0.073</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>-0.141</v>
+        <v>45.891</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>0.8879</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>-0.65</v>
+        <v>-0.004</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>0.234</v>
+        <v>0.002</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>-2.779</v>
+        <v>-1.642</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>0.0054</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="2" t="n">
-        <v>0.181</v>
-      </c>
-      <c r="C4" s="2" t="n">
-        <v>0.286</v>
-      </c>
-      <c r="D4" s="2" t="n">
-        <v>0.632</v>
-      </c>
-      <c r="E4" s="2" t="n">
-        <v>0.5276</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="2" t="n">
-        <v>0.005</v>
-      </c>
-      <c r="C5" s="2" t="n">
-        <v>0.372</v>
-      </c>
-      <c r="D5" s="2" t="n">
-        <v>0.014</v>
-      </c>
-      <c r="E5" s="2" t="n">
-        <v>0.9887</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="2" t="n">
-        <v>-0.043</v>
-      </c>
-      <c r="C6" s="2" t="n">
-        <v>0.022</v>
-      </c>
-      <c r="D6" s="2" t="n">
-        <v>-2.017</v>
-      </c>
-      <c r="E6" s="2" t="n">
-        <v>0.0437</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="2" t="n">
-        <v>0.014</v>
-      </c>
-      <c r="C7" s="2" t="n">
-        <v>0.005</v>
-      </c>
-      <c r="D7" s="2" t="n">
-        <v>2.612</v>
-      </c>
-      <c r="E7" s="2" t="n">
-        <v>0.009</v>
+        <v>0.1047</v>
       </c>
     </row>
   </sheetData>
@@ -928,33 +893,84 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>3.331</v>
+        <v>-7.397</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>0.073</v>
+        <v>23.907</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>45.891</v>
+        <v>-0.309</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>0</v>
+        <v>0.7579</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>16</v>
+        <v>6</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>-0.004</v>
+        <v>78.497</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>0.002</v>
+        <v>24.344</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>-1.642</v>
+        <v>3.225</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>0.1047</v>
+        <v>0.0019</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>14.898</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <v>23.965</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <v>0.622</v>
+      </c>
+      <c r="E4" s="2" t="n">
+        <v>0.5361</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>11.618</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>24.434</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <v>0.475</v>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>0.6358</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>3.754</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <v>0.923</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <v>4.066</v>
+      </c>
+      <c r="E6" s="2" t="n">
+        <v>0.0001</v>
       </c>
     </row>
   </sheetData>
@@ -993,84 +1009,33 @@
         <v>5</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>-7.397</v>
+        <v>109.002</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>23.907</v>
+        <v>4.677</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>-0.309</v>
+        <v>23.304</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>0.7579</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>78.497</v>
+        <v>-0.368</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>24.344</v>
+        <v>0.152</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>3.225</v>
+        <v>-2.425</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>0.0019</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="2" t="n">
-        <v>14.898</v>
-      </c>
-      <c r="C4" s="2" t="n">
-        <v>23.965</v>
-      </c>
-      <c r="D4" s="2" t="n">
-        <v>0.622</v>
-      </c>
-      <c r="E4" s="2" t="n">
-        <v>0.5361</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="2" t="n">
-        <v>11.618</v>
-      </c>
-      <c r="C5" s="2" t="n">
-        <v>24.434</v>
-      </c>
-      <c r="D5" s="2" t="n">
-        <v>0.475</v>
-      </c>
-      <c r="E5" s="2" t="n">
-        <v>0.6358</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="2" t="n">
-        <v>3.754</v>
-      </c>
-      <c r="C6" s="2" t="n">
-        <v>0.923</v>
-      </c>
-      <c r="D6" s="2" t="n">
-        <v>4.066</v>
-      </c>
-      <c r="E6" s="2" t="n">
-        <v>0.0001</v>
+        <v>0.0176</v>
       </c>
     </row>
   </sheetData>
@@ -1088,71 +1053,6 @@
   <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="2" t="n">
-        <v>109.002</v>
-      </c>
-      <c r="C2" s="2" t="n">
-        <v>4.677</v>
-      </c>
-      <c r="D2" s="2" t="n">
-        <v>23.304</v>
-      </c>
-      <c r="E2" s="2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="2" t="n">
-        <v>-0.368</v>
-      </c>
-      <c r="C3" s="2" t="n">
-        <v>0.152</v>
-      </c>
-      <c r="D3" s="2" t="n">
-        <v>-2.425</v>
-      </c>
-      <c r="E3" s="2" t="n">
-        <v>0.0176</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="false"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
-  <sheetData>
-    <row r="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>

</xml_diff>